<commit_message>
Change MC of storages
</commit_message>
<xml_diff>
--- a/SeminarPaper/Model/input_data/storages.xlsx
+++ b/SeminarPaper/Model/input_data/storages.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330470D4-8A5B-438B-9980-DD082DEE52DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22913FC4-7092-476C-A7A5-B30EF1AA4990}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t xml:space="preserve">Technology    	</t>
   </si>
@@ -54,9 +54,6 @@
     <t>AnnuityTot[EUR/MWa]</t>
   </si>
   <si>
-    <t>MC[EUR/MWhTh]</t>
-  </si>
-  <si>
     <t>eta</t>
   </si>
   <si>
@@ -66,15 +63,9 @@
     <t>disp</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.76			</t>
-  </si>
-  <si>
     <t xml:space="preserve">Battery Storage </t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.9			</t>
-  </si>
-  <si>
     <t>New Annuities seperated in Power and Energy</t>
   </si>
   <si>
@@ -103,6 +94,12 @@
   </si>
   <si>
     <t>FOMCost[EUR/MW(h)a]</t>
+  </si>
+  <si>
+    <t>MC[EUR/MWh]</t>
+  </si>
+  <si>
+    <t>MC[EUR/kWh]</t>
   </si>
 </sst>
 </file>
@@ -424,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,7 +442,7 @@
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,18 +471,15 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
       <c r="C2">
         <v>1237</v>
@@ -511,16 +505,13 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>750</v>
@@ -546,18 +537,15 @@
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -566,27 +554,36 @@
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>1220</v>
@@ -617,10 +614,21 @@
         <f>(((1+B12)^G9)/((1+B12)^G9-1))*F9+E9</f>
         <v>22565.636905448475</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <f>0.3/L9</f>
+        <v>0.39473684210526316</v>
+      </c>
+      <c r="K9" s="2">
+        <f>J9*1000</f>
+        <v>394.73684210526318</v>
+      </c>
+      <c r="L9">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>131</v>
@@ -651,16 +659,27 @@
         <f>(((1+B13)^G10)/((1+B13)^G10-1))*F10+E10</f>
         <v>732183.28471622174</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <f>0.3/L10</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K10" s="2">
+        <f>J10*1000</f>
+        <v>333.33333333333331</v>
+      </c>
+      <c r="L10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0.05</v>
       </c>

</xml_diff>